<commit_message>
Sample Sales Orders Schema
</commit_message>
<xml_diff>
--- a/Microsoft Access/Sample Databases/SalesOrdersSchema.xlsx
+++ b/Microsoft Access/Sample Databases/SalesOrdersSchema.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="1260" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="5260" yWindow="140" windowWidth="26080" windowHeight="20180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrdersSchema.txt" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="140">
   <si>
     <t>Table Name</t>
   </si>
@@ -51,268 +51,274 @@
     <t>CategoryID</t>
   </si>
   <si>
+    <t>int IDENTITY(1, 1)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>CategoryDescription</t>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Indexes for Categories</t>
+  </si>
+  <si>
+    <t>Index Name</t>
+  </si>
+  <si>
+    <t>Attributes / Field Names</t>
+  </si>
+  <si>
+    <t>PrimaryKey</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>CustFirstName</t>
+  </si>
+  <si>
+    <t>CustLastName</t>
+  </si>
+  <si>
+    <t>CustStreetAddress</t>
+  </si>
+  <si>
+    <t>CustCity</t>
+  </si>
+  <si>
+    <t>CustState</t>
+  </si>
+  <si>
+    <t>CustZipCode</t>
+  </si>
+  <si>
+    <t>CustAreaCode</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>CustPhoneNumber</t>
+  </si>
+  <si>
+    <t>Indexes for Customers</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>EmpFirstName</t>
+  </si>
+  <si>
+    <t>EmpLastName</t>
+  </si>
+  <si>
+    <t>EmpStreetAddress</t>
+  </si>
+  <si>
+    <t>EmpCity</t>
+  </si>
+  <si>
+    <t>EmpState</t>
+  </si>
+  <si>
+    <t>EmpZipCode</t>
+  </si>
+  <si>
+    <t>EmpAreaCode</t>
+  </si>
+  <si>
+    <t>EmpPhoneNumber</t>
+  </si>
+  <si>
+    <t>EmpBirthDate</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Indexes for Employees</t>
+  </si>
+  <si>
+    <t>Order_Details</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>CategoryDescription</t>
-  </si>
-  <si>
-    <t>nvarchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Indexes for Categories</t>
-  </si>
-  <si>
-    <t>Index Name</t>
-  </si>
-  <si>
-    <t>Attributes / Field Names</t>
-  </si>
-  <si>
-    <t>PrimaryKey</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>CustomerID</t>
-  </si>
-  <si>
-    <t>CustFirstName</t>
-  </si>
-  <si>
-    <t>CustLastName</t>
-  </si>
-  <si>
-    <t>CustStreetAddress</t>
-  </si>
-  <si>
-    <t>CustCity</t>
-  </si>
-  <si>
-    <t>CustState</t>
-  </si>
-  <si>
-    <t>CustZipCode</t>
-  </si>
-  <si>
-    <t>CustAreaCode</t>
-  </si>
-  <si>
-    <t>smallint</t>
-  </si>
-  <si>
-    <t>CustPhoneNumber</t>
-  </si>
-  <si>
-    <t>Indexes for Customers</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>EmployeeID</t>
-  </si>
-  <si>
-    <t>EmpFirstName</t>
-  </si>
-  <si>
-    <t>EmpLastName</t>
-  </si>
-  <si>
-    <t>EmpStreetAddress</t>
-  </si>
-  <si>
-    <t>EmpCity</t>
-  </si>
-  <si>
-    <t>EmpState</t>
-  </si>
-  <si>
-    <t>EmpZipCode</t>
-  </si>
-  <si>
-    <t>EmpAreaCode</t>
-  </si>
-  <si>
-    <t>EmpPhoneNumber</t>
-  </si>
-  <si>
-    <t>EmpBirthDate</t>
+    <t>Orders.OrderNumber</t>
+  </si>
+  <si>
+    <t>ProductNumber</t>
+  </si>
+  <si>
+    <t>Products.ProductNumber</t>
+  </si>
+  <si>
+    <t>QuotedPrice</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>QuantityOrdered</t>
+  </si>
+  <si>
+    <t>Indexes for Order_Details</t>
+  </si>
+  <si>
+    <t>OrdersOrder_Details1</t>
+  </si>
+  <si>
+    <t>ProductsOrder_Details1</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>ShipDate</t>
+  </si>
+  <si>
+    <t>Customers.CustomerID</t>
+  </si>
+  <si>
+    <t>Employees.EmployeeID</t>
+  </si>
+  <si>
+    <t>OrderTotal</t>
+  </si>
+  <si>
+    <t>Indexes for Orders</t>
+  </si>
+  <si>
+    <t>CustomersOrders1</t>
+  </si>
+  <si>
+    <t>EmployeesOrders1</t>
+  </si>
+  <si>
+    <t>Product_Vendors</t>
+  </si>
+  <si>
+    <t>VendorID</t>
+  </si>
+  <si>
+    <t>Vendors.VendorID</t>
+  </si>
+  <si>
+    <t>WholesalePrice</t>
+  </si>
+  <si>
+    <t>DaysToDeliver</t>
+  </si>
+  <si>
+    <t>Indexes for Product_Vendors</t>
+  </si>
+  <si>
+    <t>ProductsProduct_Vendors1</t>
+  </si>
+  <si>
+    <t>VendorsProduct_Vendors1</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductDescription</t>
+  </si>
+  <si>
+    <t>RetailPrice</t>
+  </si>
+  <si>
+    <t>QuantityOnHand</t>
+  </si>
+  <si>
+    <t>Categories.CategoryID</t>
+  </si>
+  <si>
+    <t>Indexes for Products</t>
+  </si>
+  <si>
+    <t>CategoriesProducts1</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>VendName</t>
+  </si>
+  <si>
+    <t>VendStreetAddress</t>
+  </si>
+  <si>
+    <t>VendCity</t>
+  </si>
+  <si>
+    <t>VendState</t>
+  </si>
+  <si>
+    <t>VendZipCode</t>
+  </si>
+  <si>
+    <t>VendPhoneNumber</t>
+  </si>
+  <si>
+    <t>VendFaxNumber</t>
+  </si>
+  <si>
+    <t>VendWebPage</t>
+  </si>
+  <si>
+    <t>nvarchar(max)</t>
+  </si>
+  <si>
+    <t>VendEMailAddress</t>
+  </si>
+  <si>
+    <t>Indexes for Vendors</t>
+  </si>
+  <si>
+    <t>ztblMonths</t>
+  </si>
+  <si>
+    <t>MonthYear</t>
+  </si>
+  <si>
+    <t>YearNumber</t>
+  </si>
+  <si>
+    <t>MonthNumber</t>
+  </si>
+  <si>
+    <t>MonthStart</t>
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Indexes for Employees</t>
-  </si>
-  <si>
-    <t>Order_Details</t>
-  </si>
-  <si>
-    <t>OrderNumber</t>
-  </si>
-  <si>
-    <t>Orders.OrderNumber</t>
-  </si>
-  <si>
-    <t>ProductNumber</t>
-  </si>
-  <si>
-    <t>Products.ProductNumber</t>
-  </si>
-  <si>
-    <t>QuotedPrice</t>
-  </si>
-  <si>
-    <t>money</t>
-  </si>
-  <si>
-    <t>QuantityOrdered</t>
-  </si>
-  <si>
-    <t>Indexes for Order_Details</t>
-  </si>
-  <si>
-    <t>OrdersOrder_Details</t>
-  </si>
-  <si>
-    <t>ProductsOrder_Details</t>
-  </si>
-  <si>
-    <t>Orders</t>
-  </si>
-  <si>
-    <t>OrderDate</t>
-  </si>
-  <si>
-    <t>ShipDate</t>
-  </si>
-  <si>
-    <t>Customers.CustomerID</t>
-  </si>
-  <si>
-    <t>Employees.EmployeeID</t>
-  </si>
-  <si>
-    <t>OrderTotal</t>
-  </si>
-  <si>
-    <t>Indexes for Orders</t>
-  </si>
-  <si>
-    <t>CustomersOrders</t>
-  </si>
-  <si>
-    <t>EmployeesOrders</t>
-  </si>
-  <si>
-    <t>Product_Vendors</t>
-  </si>
-  <si>
-    <t>VendorID</t>
-  </si>
-  <si>
-    <t>Vendors.VendorID</t>
-  </si>
-  <si>
-    <t>WholesalePrice</t>
-  </si>
-  <si>
-    <t>DaysToDeliver</t>
-  </si>
-  <si>
-    <t>Indexes for Product_Vendors</t>
-  </si>
-  <si>
-    <t>ProductsProduct_Vendors</t>
-  </si>
-  <si>
-    <t>VendorsProduct_Vendors</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>ProductName</t>
-  </si>
-  <si>
-    <t>ProductDescription</t>
-  </si>
-  <si>
-    <t>RetailPrice</t>
-  </si>
-  <si>
-    <t>QuantityOnHand</t>
-  </si>
-  <si>
-    <t>Categories.CategoryID</t>
-  </si>
-  <si>
-    <t>Indexes for Products</t>
-  </si>
-  <si>
-    <t>CategoriesProducts</t>
-  </si>
-  <si>
-    <t>Vendors</t>
-  </si>
-  <si>
-    <t>VendName</t>
-  </si>
-  <si>
-    <t>VendStreetAddress</t>
-  </si>
-  <si>
-    <t>VendCity</t>
-  </si>
-  <si>
-    <t>VendState</t>
-  </si>
-  <si>
-    <t>VendZipCode</t>
-  </si>
-  <si>
-    <t>VendPhoneNumber</t>
-  </si>
-  <si>
-    <t>VendFaxNumber</t>
-  </si>
-  <si>
-    <t>VendWebPage</t>
-  </si>
-  <si>
-    <t>nvarchar(max)</t>
-  </si>
-  <si>
-    <t>VendEMailAddress</t>
-  </si>
-  <si>
-    <t>Indexes for Vendors</t>
-  </si>
-  <si>
-    <t>ztblMonths</t>
-  </si>
-  <si>
-    <t>MonthYear</t>
-  </si>
-  <si>
-    <t>YearNumber</t>
-  </si>
-  <si>
-    <t>MonthNumber</t>
-  </si>
-  <si>
-    <t>MonthStart</t>
   </si>
   <si>
     <t>MonthEnd</t>
@@ -439,8 +445,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -468,8 +482,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,33 +818,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="A236" sqref="A236:XFD236"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -848,12 +871,6 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
@@ -879,11 +896,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" s="1" customFormat="1">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -910,29 +927,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:8" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -951,9 +968,6 @@
       <c r="D14">
         <v>4</v>
       </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
@@ -1059,11 +1073,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" s="1" customFormat="1">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1120,29 +1134,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:8" s="1" customFormat="1">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1161,9 +1175,6 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
       <c r="G38" t="s">
         <v>11</v>
       </c>
@@ -1280,11 +1291,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" t="s">
+    <row r="50" spans="1:8" s="1" customFormat="1">
+      <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1341,29 +1352,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="61" spans="1:8" s="1" customFormat="1">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1377,7 +1388,7 @@
         <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D63">
         <v>4</v>
@@ -1392,15 +1403,15 @@
         <v>11</v>
       </c>
       <c r="H63" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="B64" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D64">
         <v>4</v>
@@ -1415,15 +1426,15 @@
         <v>11</v>
       </c>
       <c r="H64" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="B65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D65">
         <v>8</v>
@@ -1434,7 +1445,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="B66" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C66" t="s">
         <v>29</v>
@@ -1453,20 +1464,20 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="1" customFormat="1">
+      <c r="A69" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1494,7 +1505,7 @@
     </row>
     <row r="75" spans="1:6">
       <c r="B75" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1504,12 +1515,12 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="B78" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1522,35 +1533,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="81" spans="1:8" s="1" customFormat="1">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C81" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="C81" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -1563,19 +1574,13 @@
       <c r="D83">
         <v>4</v>
       </c>
-      <c r="E83" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
       <c r="G83" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="B84" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
@@ -1586,7 +1591,7 @@
     </row>
     <row r="85" spans="1:8">
       <c r="B85" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C85" t="s">
         <v>43</v>
@@ -1600,7 +1605,7 @@
         <v>21</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D86">
         <v>4</v>
@@ -1609,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -1617,7 +1622,7 @@
         <v>33</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -1626,15 +1631,15 @@
         <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="B88" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C88" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D88">
         <v>8</v>
@@ -1647,20 +1652,20 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="1" customFormat="1">
+      <c r="A91" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -1675,7 +1680,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -1711,43 +1716,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
-      <c r="A102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B102" t="s">
+    <row r="102" spans="1:8" s="1" customFormat="1">
+      <c r="A102" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C102" t="s">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G102" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H102" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:8">
       <c r="B104" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C104" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D104">
         <v>4</v>
@@ -1762,15 +1767,15 @@
         <v>11</v>
       </c>
       <c r="H104" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="B105" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D105">
         <v>4</v>
@@ -1782,15 +1787,15 @@
         <v>11</v>
       </c>
       <c r="H105" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="106" spans="1:8">
       <c r="B106" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C106" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D106">
         <v>8</v>
@@ -1801,7 +1806,7 @@
     </row>
     <row r="107" spans="1:8">
       <c r="B107" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C107" t="s">
         <v>29</v>
@@ -1820,14 +1825,14 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
-      <c r="A110" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" s="1" customFormat="1">
+      <c r="A110" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1841,12 +1846,12 @@
     </row>
     <row r="112" spans="1:8">
       <c r="B112" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="B113" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -1856,12 +1861,12 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:8">
       <c r="B116" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -1871,12 +1876,12 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="119" spans="1:8">
       <c r="B119" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -1889,40 +1894,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
-      <c r="A122" t="s">
-        <v>0</v>
-      </c>
-      <c r="B122" t="s">
+    <row r="122" spans="1:8" s="1" customFormat="1">
+      <c r="A122" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C122" t="s">
-        <v>2</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C122" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F122" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G122" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H122" t="s">
+      <c r="H122" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="124" spans="1:8">
       <c r="B124" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C124" t="s">
         <v>10</v>
@@ -1930,19 +1935,13 @@
       <c r="D124">
         <v>4</v>
       </c>
-      <c r="E124" t="s">
-        <v>11</v>
-      </c>
-      <c r="F124">
-        <v>0</v>
-      </c>
       <c r="G124" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:8">
       <c r="B125" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C125" t="s">
         <v>13</v>
@@ -1953,7 +1952,7 @@
     </row>
     <row r="126" spans="1:8">
       <c r="B126" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C126" t="s">
         <v>13</v>
@@ -1964,10 +1963,10 @@
     </row>
     <row r="127" spans="1:8">
       <c r="B127" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C127" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D127">
         <v>8</v>
@@ -1978,7 +1977,7 @@
     </row>
     <row r="128" spans="1:8">
       <c r="B128" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C128" t="s">
         <v>29</v>
@@ -1995,7 +1994,7 @@
         <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D129">
         <v>4</v>
@@ -2004,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="H129" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -2014,20 +2013,20 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8">
-      <c r="A132" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" s="1" customFormat="1">
+      <c r="A132" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -2050,7 +2049,7 @@
     </row>
     <row r="137" spans="1:8">
       <c r="B137" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -2063,40 +2062,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
-      <c r="A140" t="s">
-        <v>0</v>
-      </c>
-      <c r="B140" t="s">
+    <row r="140" spans="1:8" s="1" customFormat="1">
+      <c r="A140" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C140" t="s">
-        <v>2</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="C140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F140" t="s">
+      <c r="F140" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H140" t="s">
+      <c r="H140" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="142" spans="1:8">
       <c r="B142" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C142" t="s">
         <v>10</v>
@@ -2104,16 +2103,13 @@
       <c r="D142">
         <v>4</v>
       </c>
-      <c r="E142" t="s">
-        <v>11</v>
-      </c>
       <c r="G142" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:8">
       <c r="B143" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C143" t="s">
         <v>13</v>
@@ -2124,7 +2120,7 @@
     </row>
     <row r="144" spans="1:8">
       <c r="B144" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C144" t="s">
         <v>13</v>
@@ -2135,7 +2131,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="B145" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C145" t="s">
         <v>13</v>
@@ -2146,7 +2142,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="B146" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C146" t="s">
         <v>13</v>
@@ -2157,7 +2153,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="B147" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C147" t="s">
         <v>13</v>
@@ -2168,7 +2164,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="B148" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C148" t="s">
         <v>13</v>
@@ -2179,7 +2175,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="B149" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C149" t="s">
         <v>13</v>
@@ -2190,10 +2186,10 @@
     </row>
     <row r="150" spans="1:4">
       <c r="B150" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C150" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -2201,7 +2197,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="B151" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C151" t="s">
         <v>13</v>
@@ -2217,14 +2213,14 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="A154" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" s="1" customFormat="1">
+      <c r="A154" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2238,7 +2234,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="B156" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -2248,12 +2244,12 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="B159" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2266,40 +2262,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
-      <c r="A162" t="s">
-        <v>0</v>
-      </c>
-      <c r="B162" t="s">
+    <row r="162" spans="1:8" s="1" customFormat="1">
+      <c r="A162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C162" t="s">
-        <v>2</v>
-      </c>
-      <c r="D162" t="s">
+      <c r="C162" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D162" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F162" t="s">
+      <c r="F162" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G162" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H162" t="s">
+      <c r="H162" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="164" spans="1:8">
       <c r="B164" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C164" t="s">
         <v>13</v>
@@ -2313,7 +2309,7 @@
     </row>
     <row r="165" spans="1:8">
       <c r="B165" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C165" t="s">
         <v>29</v>
@@ -2330,7 +2326,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="B166" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C166" t="s">
         <v>29</v>
@@ -2347,10 +2343,10 @@
     </row>
     <row r="167" spans="1:8">
       <c r="B167" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C167" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="D167">
         <v>8</v>
@@ -2361,10 +2357,10 @@
     </row>
     <row r="168" spans="1:8">
       <c r="B168" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C168" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="D168">
         <v>8</v>
@@ -2375,7 +2371,7 @@
     </row>
     <row r="169" spans="1:8">
       <c r="B169" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C169" t="s">
         <v>29</v>
@@ -2392,7 +2388,7 @@
     </row>
     <row r="170" spans="1:8">
       <c r="B170" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C170" t="s">
         <v>29</v>
@@ -2409,7 +2405,7 @@
     </row>
     <row r="171" spans="1:8">
       <c r="B171" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C171" t="s">
         <v>29</v>
@@ -2426,7 +2422,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="B172" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C172" t="s">
         <v>29</v>
@@ -2443,7 +2439,7 @@
     </row>
     <row r="173" spans="1:8">
       <c r="B173" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C173" t="s">
         <v>29</v>
@@ -2460,7 +2456,7 @@
     </row>
     <row r="174" spans="1:8">
       <c r="B174" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C174" t="s">
         <v>29</v>
@@ -2477,7 +2473,7 @@
     </row>
     <row r="175" spans="1:8">
       <c r="B175" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C175" t="s">
         <v>29</v>
@@ -2494,7 +2490,7 @@
     </row>
     <row r="176" spans="1:8">
       <c r="B176" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C176" t="s">
         <v>29</v>
@@ -2511,7 +2507,7 @@
     </row>
     <row r="177" spans="1:6">
       <c r="B177" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C177" t="s">
         <v>29</v>
@@ -2528,7 +2524,7 @@
     </row>
     <row r="178" spans="1:6">
       <c r="B178" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C178" t="s">
         <v>29</v>
@@ -2545,7 +2541,7 @@
     </row>
     <row r="179" spans="1:6">
       <c r="B179" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C179" t="s">
         <v>29</v>
@@ -2562,7 +2558,7 @@
     </row>
     <row r="180" spans="1:6">
       <c r="B180" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C180" t="s">
         <v>29</v>
@@ -2584,28 +2580,28 @@
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6">
-      <c r="A183" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" s="1" customFormat="1">
+      <c r="A183" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B184" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="185" spans="1:6">
       <c r="B185" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -2615,15 +2611,15 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B187" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="B188" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -2633,15 +2629,15 @@
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B190" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="191" spans="1:6">
       <c r="B191" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -2659,12 +2655,12 @@
     </row>
     <row r="194" spans="1:8">
       <c r="B194" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="195" spans="1:8">
       <c r="B195" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -2677,40 +2673,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" t="s">
-        <v>0</v>
-      </c>
-      <c r="B198" t="s">
+    <row r="198" spans="1:8" s="1" customFormat="1">
+      <c r="A198" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C198" t="s">
-        <v>2</v>
-      </c>
-      <c r="D198" t="s">
+      <c r="C198" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D198" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F198" t="s">
+      <c r="F198" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G198" t="s">
+      <c r="G198" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H198" t="s">
+      <c r="H198" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="200" spans="1:8">
       <c r="B200" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C200" t="s">
         <v>13</v>
@@ -2727,10 +2723,10 @@
     </row>
     <row r="201" spans="1:8">
       <c r="B201" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C201" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D201">
         <v>8</v>
@@ -2738,10 +2734,10 @@
     </row>
     <row r="202" spans="1:8">
       <c r="B202" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C202" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D202">
         <v>8</v>
@@ -2754,14 +2750,14 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8">
-      <c r="A205" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" s="1" customFormat="1">
+      <c r="A205" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2775,7 +2771,7 @@
     </row>
     <row r="207" spans="1:8">
       <c r="B207" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -2788,43 +2784,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
-      <c r="A210" t="s">
-        <v>0</v>
-      </c>
-      <c r="B210" t="s">
+    <row r="210" spans="1:8" s="1" customFormat="1">
+      <c r="A210" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C210" t="s">
-        <v>2</v>
-      </c>
-      <c r="D210" t="s">
+      <c r="C210" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F210" t="s">
+      <c r="F210" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G210" t="s">
+      <c r="G210" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H210" t="s">
+      <c r="H210" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="211" spans="1:8">
       <c r="A211" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="212" spans="1:8">
       <c r="B212" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C212" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D212">
         <v>8</v>
@@ -2838,10 +2834,10 @@
     </row>
     <row r="213" spans="1:8">
       <c r="B213" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C213" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D213">
         <v>8</v>
@@ -2849,7 +2845,7 @@
     </row>
     <row r="214" spans="1:8">
       <c r="B214" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C214" t="s">
         <v>29</v>
@@ -2868,25 +2864,25 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8">
-      <c r="A217" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" s="1" customFormat="1">
+      <c r="A217" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B217" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="218" spans="1:8">
       <c r="A218" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="219" spans="1:8">
       <c r="B219" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -2904,7 +2900,7 @@
     </row>
     <row r="222" spans="1:8">
       <c r="B222" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -2917,43 +2913,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
-      <c r="A225" t="s">
-        <v>0</v>
-      </c>
-      <c r="B225" t="s">
+    <row r="225" spans="1:8" s="1" customFormat="1">
+      <c r="A225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C225" t="s">
-        <v>2</v>
-      </c>
-      <c r="D225" t="s">
+      <c r="C225" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D225" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E225" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F225" t="s">
+      <c r="F225" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G225" t="s">
+      <c r="G225" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H225" t="s">
+      <c r="H225" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="226" spans="1:8">
       <c r="A226" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="227" spans="1:8">
       <c r="B227" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C227" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D227">
         <v>4</v>
@@ -2975,14 +2971,14 @@
     </row>
     <row r="229" spans="1:8">
       <c r="A229" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8">
-      <c r="A230" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" s="1" customFormat="1">
+      <c r="A230" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B230" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2996,7 +2992,7 @@
     </row>
     <row r="232" spans="1:8">
       <c r="B232" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -3010,42 +3006,42 @@
       </c>
     </row>
     <row r="235" spans="1:8">
-      <c r="A235" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8">
-      <c r="A236" t="s">
-        <v>127</v>
-      </c>
-      <c r="B236" t="s">
+      <c r="A235" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C236" t="s">
+    </row>
+    <row r="236" spans="1:8" s="1" customFormat="1">
+      <c r="A236" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D236" t="s">
+      <c r="B236" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E236" t="s">
+      <c r="C236" s="1" t="s">
         <v>131</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D237" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E237" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -3055,19 +3051,19 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B239" t="s">
         <v>20</v>
       </c>
       <c r="C239" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D239" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E239" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -3077,19 +3073,19 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B241" t="s">
         <v>32</v>
       </c>
       <c r="C241" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D241" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E241" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -3099,19 +3095,19 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B243" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C243" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D243" t="s">
         <v>45</v>
       </c>
       <c r="E243" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -3121,19 +3117,19 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B245" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C245" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D245" t="s">
         <v>45</v>
       </c>
       <c r="E245" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -3143,19 +3139,19 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B247" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C247" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D247" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E247" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -3165,19 +3161,19 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B249" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C249" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D249" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E249" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="250" spans="1:5">

</xml_diff>